<commit_message>
Updated ITA model - 2025-08-16 18:18
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801DFFC6-978D-473E-8FA4-D07342F89D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC673B1-FB36-42E4-901D-18DD441F412D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1245,7 +1245,7 @@
   <dimension ref="C3:X43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="C42" sqref="C42:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1387,7 +1387,7 @@
       <c r="E11" t="s">
         <v>64</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>8.76</v>
       </c>
       <c r="P11" t="s">

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 00:07
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB65D116-CE0B-4A73-9EBA-1A2B1F6633DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61489740-49F3-4F4F-9A7B-48AA7A9A2197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="74">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -244,13 +244,22 @@
     <t>pset_ci</t>
   </si>
   <si>
-    <t>solar,wind,coal,gas,nuclear,hydro</t>
-  </si>
-  <si>
     <t>attrib_cond</t>
   </si>
   <si>
     <t>-pasti</t>
+  </si>
+  <si>
+    <t>solar,wind,coal,gas,nuclear,hydro,bioenergy</t>
+  </si>
+  <si>
+    <t>life</t>
+  </si>
+  <si>
+    <t>-life</t>
+  </si>
+  <si>
+    <t>coal,gas,nuclear,bioenergy</t>
   </si>
 </sst>
 </file>
@@ -1251,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C4:X48"/>
+  <dimension ref="C4:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1990,7 +1999,7 @@
         <v>26</v>
       </c>
       <c r="E47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F47" t="s">
         <v>67</v>
@@ -2004,10 +2013,24 @@
         <v>2025</v>
       </c>
       <c r="E48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48" t="s">
         <v>70</v>
       </c>
-      <c r="F48" t="s">
-        <v>68</v>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="C49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49">
+        <v>40</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>